<commit_message>
feat: remove category resource
</commit_message>
<xml_diff>
--- a/public/templates/import.xlsx
+++ b/public/templates/import.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -28,16 +28,13 @@
     <t xml:space="preserve">nome</t>
   </si>
   <si>
-    <t xml:space="preserve">e categoria?</t>
-  </si>
-  <si>
     <t xml:space="preserve">definicao</t>
   </si>
   <si>
     <t xml:space="preserve">notas</t>
   </si>
   <si>
-    <t xml:space="preserve">objeto superior</t>
+    <t xml:space="preserve">verbete superior</t>
   </si>
   <si>
     <t xml:space="preserve">variacoes</t>
@@ -58,9 +55,6 @@
     <t xml:space="preserve">abrasão</t>
   </si>
   <si>
-    <t xml:space="preserve">0</t>
-  </si>
-  <si>
     <t xml:space="preserve">Dano ocasionado pela fricção entre os materiais ou com algum material abrasivo, como a poeira, que resulta no desgaste das superfícies e mídias nas obras em papel.</t>
   </si>
   <si>
@@ -92,9 +86,6 @@
   </si>
   <si>
     <t xml:space="preserve">Danos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
   </si>
 </sst>
 </file>
@@ -192,27 +183,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="40.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="29.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="39.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="57.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="43.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="111.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="40.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="39.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="57.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="43.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="111.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -240,85 +231,70 @@
       <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="B2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="0" t="s">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="0" t="s">
+      <c r="F3" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="0" t="s">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
feat(forms): change default labels
</commit_message>
<xml_diff>
--- a/public/templates/import.xlsx
+++ b/public/templates/import.xlsx
@@ -25,7 +25,7 @@
     <t xml:space="preserve">id</t>
   </si>
   <si>
-    <t xml:space="preserve">nome</t>
+    <t xml:space="preserve">termo</t>
   </si>
   <si>
     <t xml:space="preserve">definicao</t>
@@ -34,19 +34,19 @@
     <t xml:space="preserve">notas</t>
   </si>
   <si>
-    <t xml:space="preserve">verbete superior</t>
-  </si>
-  <si>
-    <t xml:space="preserve">variacoes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">traducoes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">verbetes relacionados</t>
-  </si>
-  <si>
-    <t xml:space="preserve">referencias</t>
+    <t xml:space="preserve">termo superior</t>
+  </si>
+  <si>
+    <t xml:space="preserve">formas variantes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">termos equivalentes em outros idiomas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ver tambem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fontes</t>
   </si>
   <si>
     <t xml:space="preserve">abrasao</t>
@@ -186,10 +186,10 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.17"/>

</xml_diff>

<commit_message>
feat: allow import and export of concept position
</commit_message>
<xml_diff>
--- a/public/templates/import.xlsx
+++ b/public/templates/import.xlsx
@@ -13,14 +13,14 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t xml:space="preserve">fontes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">posicao</t>
   </si>
   <si>
     <t xml:space="preserve">abrasao</t>
@@ -161,8 +164,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -183,122 +198,133 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="40.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="39.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="57.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="43.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="111.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="40.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="29.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="39.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="43.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="112.01"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="0" t="s">
+    <row r="2" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="D2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="E2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="G2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="H2" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="I2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="3" t="n">
+        <v>2</v>
+      </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="0" t="s">
+    <row r="3" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>16</v>
+      <c r="J3" s="3" t="n">
+        <v>1</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>21</v>
+    <row r="4" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="3" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>